<commit_message>
Adding new read data from excelsheet and pass it into datadriver
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Data.xlsx
+++ b/src/main/java/resources/Data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium4\Selenuim_Framework_Design\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6866091D-3310-45A4-92FB-D440A9EF91BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80A9C8B-F58C-42BE-8D2B-EC768D8AA06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="5640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4140" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData1" sheetId="1" r:id="rId1"/>
-    <sheet name="sample" sheetId="2" r:id="rId2"/>
+    <sheet name="TestData2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Login</t>
   </si>
@@ -59,13 +59,40 @@
   </si>
   <si>
     <t>password1</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>dexcomnew98@gmail.com</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>user@gmail.com</t>
+  </si>
+  <si>
+    <t>User123#</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Incorrect email or password.</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +100,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,13 +132,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,13 +423,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -466,12 +512,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD0B2CE-EFD8-4757-A666-C4F23DC15B72}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{095C61E7-8098-4CBE-A495-F233546E58C0}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{24616355-1C25-48C2-BA4C-595948992158}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{2782500C-1A81-426A-9C29-9B62E1BE5367}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update method and remove exception
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Data.xlsx
+++ b/src/main/java/resources/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium4\Selenuim_Framework_Design\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80A9C8B-F58C-42BE-8D2B-EC768D8AA06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233C5929-D02D-4D35-970E-8693B0888AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4140" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Login</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Incorrect</t>
+  </si>
+  <si>
+    <t>Login Successfully.</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,10 +145,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -512,10 +523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD0B2CE-EFD8-4757-A666-C4F23DC15B72}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,23 +547,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -566,14 +577,26 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{095C61E7-8098-4CBE-A495-F233546E58C0}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{24616355-1C25-48C2-BA4C-595948992158}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{2782500C-1A81-426A-9C29-9B62E1BE5367}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{095C61E7-8098-4CBE-A495-F233546E58C0}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{24616355-1C25-48C2-BA4C-595948992158}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{2782500C-1A81-426A-9C29-9B62E1BE5367}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{53B79632-AFEC-4745-B79F-925C883296DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
push updating files 2014
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Data.xlsx
+++ b/src/main/java/resources/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium4\Selenuim_Framework_Design\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233C5929-D02D-4D35-970E-8693B0888AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EFA6B2-0EF1-403E-91BA-2F17BB2A9F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,7 +88,7 @@
     <t>Incorrect</t>
   </si>
   <si>
-    <t>Login Successfully.</t>
+    <t>Login Successfully</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding allure report and fluent wait
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Data.xlsx
+++ b/src/main/java/resources/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium4\Selenuim_Framework_Design\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EFA6B2-0EF1-403E-91BA-2F17BB2A9F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4E0458-BC16-4A6D-A5B9-15DD231BF262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>